<commit_message>
update: pebaruan sistem setoran
</commit_message>
<xml_diff>
--- a/DATA TUNGGAKAN SANTRI PUTRA 2021-2022.xlsx
+++ b/DATA TUNGGAKAN SANTRI PUTRA 2021-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrome\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABBF480-B8A7-4C04-995F-ADE4A55D5419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362E404B-6713-4149-9449-DF965DD81855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{E0BFB4A3-1715-401E-BBD6-FB1E99669929}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E0BFB4A3-1715-401E-BBD6-FB1E99669929}"/>
   </bookViews>
   <sheets>
     <sheet name="MA" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="SMP" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MA!$A$1:$G$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MA!$A$1:$F$105</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MTs!$A$1:$G$66</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SMK!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">SMP!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="218">
   <si>
     <t>ALFIN SILAHI</t>
   </si>
@@ -694,13 +696,7 @@
     <t>082211136708</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>082245497867</t>
-  </si>
-  <si>
-    <t>08233</t>
   </si>
 </sst>
 </file>
@@ -708,8 +704,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -744,7 +740,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -752,44 +748,23 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1105,30 +1080,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B124F51-73F2-4E4F-ADEA-AA701BBCA26E}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
@@ -1141,281 +1115,1765 @@
       <c r="D1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1200000</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1148000</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1220000</v>
+      </c>
+      <c r="F3" s="7">
+        <v>448000</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1080000</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1109000</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="7">
+        <v>600000</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1798000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1109000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1109000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F9" s="7">
+        <v>989000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>698000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>617000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F12" s="7">
+        <v>580000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F13" s="7">
+        <v>517000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F14" s="7">
+        <v>448000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F15" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F16" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F17" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F18" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F19" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E20" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F20" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F21" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F22" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E23" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F23" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E24" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F24" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E25" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F25" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E26" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F26" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F27" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F28" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F29" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F30" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F31" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F32" s="7">
+        <v>243000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F33" s="7">
+        <v>216000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E35" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E44" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F45" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E48" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E50" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E51" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F51" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F52" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F53" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F54" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F55" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" s="7">
+        <v>300000</v>
+      </c>
+      <c r="F56" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="7">
+        <v>0</v>
+      </c>
+      <c r="F57" s="7">
+        <v>928000</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7">
+        <v>928000</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0</v>
+      </c>
+      <c r="F59" s="7">
+        <v>813000</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0</v>
+      </c>
+      <c r="F60" s="7">
+        <v>808000</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7">
+        <v>580000</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7">
+        <v>562000</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" s="7">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7">
+        <v>509000</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0</v>
+      </c>
+      <c r="F64" s="7">
+        <v>361000</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="6"/>
+      <c r="E65" s="7">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7">
+        <v>306000</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" t="s">
+        <v>64</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0</v>
+      </c>
+      <c r="F66" s="7">
+        <v>303000</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" t="s">
+        <v>64</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0</v>
+      </c>
+      <c r="F69" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E70" s="7">
+        <v>0</v>
+      </c>
+      <c r="F70" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" t="s">
+        <v>64</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E71" s="7">
+        <v>0</v>
+      </c>
+      <c r="F71" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" t="s">
+        <v>64</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E72" s="7">
+        <v>0</v>
+      </c>
+      <c r="F72" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" t="s">
+        <v>64</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0</v>
+      </c>
+      <c r="F73" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" t="s">
+        <v>64</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0</v>
+      </c>
+      <c r="F74" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>83</v>
+      </c>
+      <c r="C75" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E75" s="7">
+        <v>0</v>
+      </c>
+      <c r="F75" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>84</v>
+      </c>
+      <c r="C76" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0</v>
+      </c>
+      <c r="F76" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" t="s">
+        <v>88</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E77" s="7">
+        <v>0</v>
+      </c>
+      <c r="F77" s="7">
+        <v>296000</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E78" s="7">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7">
+        <v>266000</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" t="s">
+        <v>64</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E79" s="7">
+        <v>0</v>
+      </c>
+      <c r="F79" s="7">
+        <v>266000</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" t="s">
+        <v>82</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0</v>
+      </c>
+      <c r="F80" s="7">
+        <v>266000</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="1">
-        <v>246000</v>
-      </c>
-      <c r="G2" s="2">
-        <f t="shared" ref="G2:G13" si="0">E2+F2</f>
-        <v>246000</v>
-      </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E81" s="7">
+        <v>0</v>
+      </c>
+      <c r="F81" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" t="s">
+        <v>89</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0</v>
+      </c>
+      <c r="F82" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E83" s="7">
+        <v>0</v>
+      </c>
+      <c r="F83" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E84" s="7">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>31</v>
+      </c>
+      <c r="C85" t="s">
+        <v>49</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E85" s="7">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E86" s="7">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87" t="s">
+        <v>49</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E87" s="7">
+        <v>0</v>
+      </c>
+      <c r="F87" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>49</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E88" s="7">
+        <v>0</v>
+      </c>
+      <c r="F88" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>69</v>
+      </c>
+      <c r="C89" t="s">
+        <v>49</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E89" s="7">
+        <v>0</v>
+      </c>
+      <c r="F89" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" t="s">
+        <v>49</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E90" s="7">
+        <v>0</v>
+      </c>
+      <c r="F90" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
+        <v>28</v>
+      </c>
+      <c r="C91" t="s">
+        <v>49</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E91" s="7">
+        <v>0</v>
+      </c>
+      <c r="F91" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>73</v>
+      </c>
+      <c r="C92" t="s">
+        <v>82</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E92" s="7">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B93" t="s">
+        <v>77</v>
+      </c>
+      <c r="C93" t="s">
+        <v>82</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E93" s="7">
+        <v>0</v>
+      </c>
+      <c r="F93" s="7">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>37</v>
+      </c>
+      <c r="C94" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E94" s="7">
+        <v>0</v>
+      </c>
+      <c r="F94" s="7">
+        <v>243000</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
+        <v>33</v>
+      </c>
+      <c r="C95" t="s">
+        <v>49</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E95" s="7">
+        <v>0</v>
+      </c>
+      <c r="F95" s="7">
+        <v>241000</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>63</v>
+      </c>
+      <c r="C96" t="s">
+        <v>49</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E96" s="7">
+        <v>0</v>
+      </c>
+      <c r="F96" s="7">
+        <v>241000</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>89</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E97" s="7">
+        <v>0</v>
+      </c>
+      <c r="F97" s="7">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" t="s">
+        <v>49</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E98" s="7">
+        <v>0</v>
+      </c>
+      <c r="F98" s="7">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>13</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E99" s="7">
+        <v>0</v>
+      </c>
+      <c r="F99" s="7">
+        <v>216000</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B100" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" t="s">
+        <v>82</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E100" s="7">
+        <v>0</v>
+      </c>
+      <c r="F100" s="7">
+        <v>216000</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>40</v>
+      </c>
+      <c r="C101" t="s">
+        <v>49</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E101" s="7">
+        <v>0</v>
+      </c>
+      <c r="F101" s="7">
+        <v>204000</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C102" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D102" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="1">
+      <c r="E102" s="7">
+        <v>0</v>
+      </c>
+      <c r="F102" s="7">
         <v>196000</v>
       </c>
-      <c r="G3" s="2">
-        <f t="shared" si="0"/>
-        <v>196000</v>
-      </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B103" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="1">
-        <v>246000</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>246000</v>
-      </c>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="1">
-        <v>240000</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>240000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="1">
-        <v>928000</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>928000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="1">
-        <v>300000</v>
-      </c>
-      <c r="F7" s="1">
-        <v>698000</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>998000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C103" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="1">
-        <v>300000</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1798000</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>2098000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="1">
-        <v>300000</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="D103" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F10" s="1">
+      <c r="E103" s="7">
+        <v>0</v>
+      </c>
+      <c r="F103" s="7">
         <v>147000</v>
       </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>147000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="1">
-        <v>246000</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>246000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E12" s="1">
-        <v>300000</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="1">
-        <v>509000</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>509000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
-        <v>217</v>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B104" t="s">
+        <v>42</v>
+      </c>
+      <c r="C104" t="s">
+        <v>49</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E104" s="7">
+        <v>0</v>
+      </c>
+      <c r="F104" s="7">
+        <v>134000</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B105" t="s">
+        <v>59</v>
+      </c>
+      <c r="C105" t="s">
+        <v>64</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E105" s="7">
+        <v>0</v>
+      </c>
+      <c r="F105" s="7">
+        <v>115000</v>
       </c>
     </row>
   </sheetData>
@@ -1429,24 +2887,24 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B2" sqref="B2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
@@ -1470,7 +2928,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1488,7 +2946,7 @@
         <v>216000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -1509,7 +2967,7 @@
         <v>596000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -1524,7 +2982,7 @@
         <v>306000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1542,7 +3000,7 @@
         <v>266000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -1563,7 +3021,7 @@
         <v>1409000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1581,7 +3039,7 @@
         <v>596000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1599,7 +3057,7 @@
         <v>813000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -1626,25 +3084,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412C6E49-1612-4EA9-8167-B7E183DEF6B3}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="89" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="B63" sqref="B2:F63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
@@ -1668,7 +3126,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1690,7 +3148,7 @@
         <v>880000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1711,7 +3169,7 @@
         <v>580000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1735,7 +3193,7 @@
         <v>1409000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1756,7 +3214,7 @@
         <v>928000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1780,7 +3238,7 @@
         <v>516000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1801,7 +3259,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1822,7 +3280,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1843,7 +3301,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1864,7 +3322,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1885,7 +3343,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1903,7 +3361,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1921,7 +3379,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1942,7 +3400,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1963,7 +3421,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1984,7 +3442,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2005,7 +3463,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2029,7 +3487,7 @@
         <v>2348000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2050,7 +3508,7 @@
         <v>303000</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2071,7 +3529,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2092,7 +3550,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2113,7 +3571,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2134,7 +3592,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2155,7 +3613,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2177,7 +3635,7 @@
         <v>596000</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2198,7 +3656,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2222,7 +3680,7 @@
         <v>596000</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2246,7 +3704,7 @@
         <v>596000</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2267,7 +3725,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2288,7 +3746,7 @@
         <v>296000</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2309,7 +3767,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2333,7 +3791,7 @@
         <v>917000</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2354,7 +3812,7 @@
         <v>266000</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2375,7 +3833,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2399,7 +3857,7 @@
         <v>2189000</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2420,7 +3878,7 @@
         <v>808000</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2441,7 +3899,7 @@
         <v>562000</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2462,7 +3920,7 @@
         <v>361000</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2483,7 +3941,7 @@
         <v>204000</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2504,7 +3962,7 @@
         <v>246000</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2528,7 +3986,7 @@
         <v>546000</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2552,7 +4010,7 @@
         <v>546000</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2576,7 +4034,7 @@
         <v>546000</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2597,7 +4055,7 @@
         <v>246000</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2621,7 +4079,7 @@
         <v>546000</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2642,7 +4100,7 @@
         <v>246000</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2663,7 +4121,7 @@
         <v>246000</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2687,7 +4145,7 @@
         <v>546000</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2711,7 +4169,7 @@
         <v>546000</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2732,7 +4190,7 @@
         <v>246000</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2753,7 +4211,7 @@
         <v>246000</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2777,7 +4235,7 @@
         <v>546000</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2798,7 +4256,7 @@
         <v>246000</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -2822,7 +4280,7 @@
         <v>543000</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -2843,7 +4301,7 @@
         <v>243000</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -2864,7 +4322,7 @@
         <v>241000</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -2885,7 +4343,7 @@
         <v>241000</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -2906,7 +4364,7 @@
         <v>240000</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -2927,7 +4385,7 @@
         <v>134000</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -2948,7 +4406,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -2969,7 +4427,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -2987,7 +4445,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -3008,17 +4466,17 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -3034,573 +4492,377 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B8C21A-2285-4F69-9405-90B547B223DA}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="A1:G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B2:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="E2" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F2" s="1">
         <v>448000</v>
       </c>
-      <c r="G2" s="11">
-        <f>E2+F2</f>
-        <v>748000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="4">
         <v>1200000</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="1">
         <v>448000</v>
       </c>
-      <c r="G3" s="11">
-        <f t="shared" ref="G3:G23" si="0">E3+F3</f>
-        <v>1648000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F4" s="10">
+      <c r="E4" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F4" s="1">
         <v>296000</v>
       </c>
-      <c r="G4" s="11">
-        <f t="shared" si="0"/>
-        <v>596000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="11">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="F5" s="1">
         <v>296000</v>
       </c>
-      <c r="G5" s="11">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="1">
         <v>296000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="8" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="11">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="D7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="1">
         <v>296000</v>
       </c>
-      <c r="G6" s="11">
-        <f t="shared" si="0"/>
-        <v>296000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0</v>
-      </c>
-      <c r="F7" s="10">
-        <v>296000</v>
-      </c>
-      <c r="G7" s="11">
-        <f t="shared" si="0"/>
-        <v>296000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="E8" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F8" s="1">
         <v>989000</v>
       </c>
-      <c r="G8" s="11">
-        <f t="shared" si="0"/>
-        <v>1289000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="E9" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="E9" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F9" s="1">
         <v>517000</v>
       </c>
-      <c r="G9" s="11">
-        <f t="shared" si="0"/>
-        <v>817000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="11">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="F10" s="1">
         <v>216000</v>
       </c>
-      <c r="G10" s="11">
-        <f t="shared" si="0"/>
-        <v>216000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10">
-        <v>246000</v>
-      </c>
-      <c r="G11" s="11">
-        <f t="shared" si="0"/>
-        <v>246000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="F11" s="1">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F12" s="10">
-        <v>246000</v>
-      </c>
-      <c r="G12" s="11">
-        <f t="shared" si="0"/>
-        <v>546000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="E12" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E13" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F13" s="10">
-        <v>246000</v>
-      </c>
-      <c r="G13" s="11">
-        <f t="shared" si="0"/>
-        <v>546000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="E13" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F13" s="1">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E14" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F14" s="10">
-        <v>246000</v>
-      </c>
-      <c r="G14" s="11">
-        <f t="shared" si="0"/>
-        <v>546000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="E14" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="E15" s="11">
-        <v>0</v>
-      </c>
-      <c r="F15" s="10">
-        <v>246000</v>
-      </c>
-      <c r="G15" s="11">
-        <f t="shared" si="0"/>
-        <v>246000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="D15" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F15" s="1">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E16" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F16" s="10">
-        <v>246000</v>
-      </c>
-      <c r="G16" s="11">
-        <f t="shared" si="0"/>
-        <v>546000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="E16" s="4">
+        <v>300000</v>
+      </c>
+      <c r="F16" s="1">
+        <v>246000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="11">
-        <v>0</v>
-      </c>
-      <c r="F17" s="10">
+      <c r="F17" s="1">
         <v>266000</v>
       </c>
-      <c r="G17" s="11">
-        <f t="shared" si="0"/>
-        <v>266000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>17</v>
-      </c>
-      <c r="B18" s="8" t="s">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E18" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>18</v>
-      </c>
-      <c r="B19" s="8" t="s">
+      <c r="E18" s="4">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E19" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>19</v>
-      </c>
-      <c r="B20" s="8" t="s">
+      <c r="E19" s="4">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" t="s">
         <v>118</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0</v>
-      </c>
-      <c r="G20" s="11">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="E20" s="4">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F21" s="11">
-        <v>0</v>
-      </c>
-      <c r="G21" s="11">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="E21" s="4">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" t="s">
         <v>118</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E22" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F22" s="11">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="E22" s="4">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E23" s="10">
-        <v>300000</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
-        <f t="shared" si="0"/>
+      <c r="E23" s="4">
         <v>300000</v>
       </c>
     </row>

</xml_diff>